<commit_message>
Working amend function as 2.0.4 version
</commit_message>
<xml_diff>
--- a/config/tablesSchema.xlsx
+++ b/config/tablesSchema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\trasys\EFSA\workspace\tse-reporting-tool\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panos\Documents\Git\CRI\EFSA\tse-reporting-tool\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB58F2AF-D206-4634-AE49-EF8C91D18949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8095B043-A461-4890-B64A-A7B1A7B04176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="600" windowWidth="28800" windowHeight="15600" tabRatio="690" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="690" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -27,24 +27,11 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">SummarizedInformation!$A$2:$E$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1714" uniqueCount="490">
   <si>
     <t>Type</t>
   </si>
@@ -1505,6 +1492,15 @@
   </si>
   <si>
     <t>2.0</t>
+  </si>
+  <si>
+    <t>aggregatorId</t>
+  </si>
+  <si>
+    <t>isAggregated</t>
+  </si>
+  <si>
+    <t>isAmended</t>
   </si>
 </sst>
 </file>
@@ -1646,7 +1642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1671,6 +1667,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3166,8 +3163,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:S13" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
-  <autoFilter ref="A1:S13" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:S17" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
+  <autoFilter ref="A1:S17" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id" dataDxfId="98"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="code" dataDxfId="97"/>
@@ -3194,8 +3191,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table2" displayName="Table2" ref="A1:S42" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
-  <autoFilter ref="A1:S42" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table2" displayName="Table2" ref="A1:S43" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
+  <autoFilter ref="A1:S43" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S43">
     <sortCondition ref="R1:R43"/>
   </sortState>
@@ -3629,25 +3626,25 @@
       <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="14" width="14.140625" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.5859375" customWidth="1"/>
+    <col min="2" max="2" width="26.41015625" customWidth="1"/>
+    <col min="3" max="3" width="12.29296875" customWidth="1"/>
+    <col min="4" max="4" width="18.29296875" customWidth="1"/>
+    <col min="5" max="5" width="35.29296875" customWidth="1"/>
+    <col min="6" max="6" width="14.703125" customWidth="1"/>
+    <col min="7" max="7" width="23.87890625" customWidth="1"/>
+    <col min="8" max="8" width="14.1171875" customWidth="1"/>
+    <col min="9" max="9" width="15.87890625" customWidth="1"/>
+    <col min="10" max="10" width="12.5859375" customWidth="1"/>
+    <col min="11" max="11" width="12.703125" customWidth="1"/>
+    <col min="12" max="14" width="14.1171875" customWidth="1"/>
+    <col min="15" max="15" width="14.703125" customWidth="1"/>
+    <col min="16" max="16" width="14.1171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -3706,7 +3703,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>136</v>
       </c>
@@ -3739,7 +3736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>137</v>
       </c>
@@ -3772,7 +3769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -3824,24 +3821,24 @@
       <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.28515625" customWidth="1"/>
-    <col min="13" max="14" width="14.140625" customWidth="1"/>
-    <col min="15" max="16" width="14.7109375" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.87890625" customWidth="1"/>
+    <col min="3" max="3" width="9.41015625" customWidth="1"/>
+    <col min="4" max="4" width="20.703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.41015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.29296875" customWidth="1"/>
+    <col min="7" max="7" width="23.87890625" customWidth="1"/>
+    <col min="8" max="8" width="12.703125" customWidth="1"/>
+    <col min="9" max="9" width="10.5859375" customWidth="1"/>
+    <col min="11" max="11" width="12.87890625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.29296875" customWidth="1"/>
+    <col min="13" max="14" width="14.1171875" customWidth="1"/>
+    <col min="15" max="16" width="14.703125" customWidth="1"/>
+    <col min="17" max="17" width="14.1171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -3900,7 +3897,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>117</v>
       </c>
@@ -3935,7 +3932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>413</v>
       </c>
@@ -3985,7 +3982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>120</v>
       </c>
@@ -4023,7 +4020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>122</v>
       </c>
@@ -4061,7 +4058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>124</v>
       </c>
@@ -4099,7 +4096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>475</v>
       </c>
@@ -4137,7 +4134,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>126</v>
       </c>
@@ -4175,7 +4172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>129</v>
       </c>
@@ -4213,7 +4210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>132</v>
       </c>
@@ -4251,7 +4248,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>476</v>
       </c>
@@ -4289,7 +4286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>330</v>
       </c>
@@ -4328,7 +4325,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>328</v>
       </c>
@@ -4367,7 +4364,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>329</v>
       </c>
@@ -4406,7 +4403,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A15" s="5" t="s">
         <v>479</v>
       </c>
@@ -4455,37 +4452,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="62.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="33.42578125" customWidth="1"/>
-    <col min="14" max="14" width="38.85546875" customWidth="1"/>
-    <col min="15" max="15" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.5859375" customWidth="1"/>
+    <col min="3" max="3" width="10.703125" customWidth="1"/>
+    <col min="4" max="4" width="18.29296875" customWidth="1"/>
+    <col min="5" max="5" width="62.29296875" customWidth="1"/>
+    <col min="6" max="6" width="13.5859375" customWidth="1"/>
+    <col min="7" max="7" width="23.87890625" customWidth="1"/>
+    <col min="8" max="8" width="14.1171875" customWidth="1"/>
+    <col min="9" max="9" width="10.5859375" customWidth="1"/>
+    <col min="10" max="10" width="10.29296875" customWidth="1"/>
+    <col min="11" max="11" width="14.41015625" customWidth="1"/>
+    <col min="12" max="12" width="14.1171875" customWidth="1"/>
+    <col min="13" max="13" width="33.41015625" customWidth="1"/>
+    <col min="14" max="14" width="38.87890625" customWidth="1"/>
+    <col min="15" max="15" width="35.29296875" customWidth="1"/>
     <col min="16" max="16" width="22" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.1171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -4544,7 +4541,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>166</v>
       </c>
@@ -4592,7 +4589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>167</v>
       </c>
@@ -4640,7 +4637,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>183</v>
       </c>
@@ -4678,7 +4675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A5" s="5" t="s">
         <v>117</v>
       </c>
@@ -4725,7 +4722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>177</v>
       </c>
@@ -4748,7 +4745,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>315</v>
       </c>
@@ -4778,7 +4775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>239</v>
       </c>
@@ -4809,7 +4806,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>386</v>
       </c>
@@ -4837,7 +4834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>387</v>
       </c>
@@ -4865,7 +4862,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>245</v>
       </c>
@@ -4901,7 +4898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>240</v>
       </c>
@@ -4937,7 +4934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>368</v>
       </c>
@@ -4965,6 +4962,129 @@
         <v>5</v>
       </c>
       <c r="S13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>488</v>
+      </c>
+      <c r="B14" t="s">
+        <v>488</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="F14" t="s">
+        <v>174</v>
+      </c>
+      <c r="H14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" t="s">
+        <v>5</v>
+      </c>
+      <c r="M14" s="10"/>
+      <c r="Q14" t="s">
+        <v>5</v>
+      </c>
+      <c r="S14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>487</v>
+      </c>
+      <c r="B15" t="s">
+        <v>487</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="F15" t="s">
+        <v>174</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" t="s">
+        <v>5</v>
+      </c>
+      <c r="M15" s="10"/>
+      <c r="Q15" t="s">
+        <v>5</v>
+      </c>
+      <c r="S15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>244</v>
+      </c>
+      <c r="B16" t="s">
+        <v>244</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="F16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" t="s">
+        <v>5</v>
+      </c>
+      <c r="M16" s="10"/>
+      <c r="Q16" t="s">
+        <v>5</v>
+      </c>
+      <c r="S16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.5">
+      <c r="A17" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" t="s">
+        <v>370</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="Q17" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4979,37 +5099,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:S42"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5859375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.41015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5859375" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="68.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="74.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="78.42578125" customWidth="1"/>
-    <col min="14" max="14" width="45.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.41015625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="68.29296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.29296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="74.703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="78.41015625" customWidth="1"/>
+    <col min="14" max="14" width="45.1171875" customWidth="1"/>
     <col min="15" max="15" width="52" customWidth="1"/>
-    <col min="16" max="16" width="71.28515625" customWidth="1"/>
+    <col min="16" max="16" width="71.29296875" customWidth="1"/>
     <col min="17" max="17" width="20" customWidth="1"/>
-    <col min="19" max="19" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.87890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -5068,7 +5188,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -5109,7 +5229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -5159,7 +5279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -5206,7 +5326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -5250,7 +5370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -5294,7 +5414,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>379</v>
       </c>
@@ -5341,7 +5461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -5394,7 +5514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>92</v>
       </c>
@@ -5447,7 +5567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -5497,7 +5617,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A11" s="12" t="s">
         <v>392</v>
       </c>
@@ -5529,7 +5649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -5567,7 +5687,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -5605,7 +5725,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -5643,7 +5763,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -5684,7 +5804,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -5722,7 +5842,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -5760,7 +5880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>265</v>
       </c>
@@ -5801,7 +5921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>262</v>
       </c>
@@ -5842,7 +5962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -5874,7 +5994,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -5906,7 +6026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>343</v>
       </c>
@@ -5932,7 +6052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>84</v>
       </c>
@@ -5964,7 +6084,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -5999,7 +6119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>177</v>
       </c>
@@ -6019,7 +6139,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -6051,7 +6171,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -6080,7 +6200,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -6115,7 +6235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>172</v>
       </c>
@@ -6135,7 +6255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -6170,7 +6290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>95</v>
       </c>
@@ -6202,7 +6322,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>76</v>
       </c>
@@ -6234,7 +6354,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -6269,7 +6389,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>97</v>
       </c>
@@ -6298,7 +6418,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -6330,7 +6450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>399</v>
       </c>
@@ -6359,7 +6479,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -6394,7 +6514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -6426,7 +6546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -6461,7 +6581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>222</v>
       </c>
@@ -6487,7 +6607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -6522,7 +6642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
         <v>178</v>
       </c>
@@ -6539,6 +6659,29 @@
         <v>4</v>
       </c>
       <c r="Q42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="A43" t="s">
+        <v>489</v>
+      </c>
+      <c r="B43" t="s">
+        <v>489</v>
+      </c>
+      <c r="F43" t="s">
+        <v>174</v>
+      </c>
+      <c r="H43" t="s">
+        <v>4</v>
+      </c>
+      <c r="I43" t="s">
+        <v>4</v>
+      </c>
+      <c r="J43" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q43" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6556,33 +6699,33 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.85546875" customWidth="1"/>
-    <col min="5" max="5" width="56.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.41015625" customWidth="1"/>
+    <col min="3" max="3" width="14.41015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.87890625" customWidth="1"/>
+    <col min="5" max="5" width="56.703125" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="143.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="82.85546875" customWidth="1"/>
-    <col min="10" max="10" width="52.140625" customWidth="1"/>
-    <col min="11" max="11" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46.140625" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" customWidth="1"/>
-    <col min="14" max="14" width="38.7109375" customWidth="1"/>
-    <col min="15" max="16" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="23.87890625" customWidth="1"/>
+    <col min="8" max="8" width="143.1171875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="82.87890625" customWidth="1"/>
+    <col min="10" max="10" width="52.1171875" customWidth="1"/>
+    <col min="11" max="11" width="29.29296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="46.1171875" customWidth="1"/>
+    <col min="13" max="13" width="29.703125" customWidth="1"/>
+    <col min="14" max="14" width="38.703125" customWidth="1"/>
+    <col min="15" max="16" width="22.87890625" customWidth="1"/>
     <col min="17" max="17" width="20" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" customWidth="1"/>
+    <col min="19" max="19" width="10.1171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -6641,7 +6784,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>410</v>
       </c>
@@ -6682,7 +6825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -6717,7 +6860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -6767,7 +6910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>379</v>
       </c>
@@ -6811,7 +6954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -6852,7 +6995,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>190</v>
       </c>
@@ -6890,7 +7033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>201</v>
       </c>
@@ -6926,7 +7069,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>205</v>
       </c>
@@ -6961,7 +7104,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>274</v>
       </c>
@@ -6996,7 +7139,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>271</v>
       </c>
@@ -7031,7 +7174,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>213</v>
       </c>
@@ -7072,7 +7215,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>194</v>
       </c>
@@ -7115,7 +7258,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>208</v>
       </c>
@@ -7153,7 +7296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>278</v>
       </c>
@@ -7191,7 +7334,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>282</v>
       </c>
@@ -7226,7 +7369,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>277</v>
       </c>
@@ -7267,7 +7410,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>287</v>
       </c>
@@ -7302,7 +7445,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>290</v>
       </c>
@@ -7337,7 +7480,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>220</v>
       </c>
@@ -7357,7 +7500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>172</v>
       </c>
@@ -7377,7 +7520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>343</v>
       </c>
@@ -7417,32 +7560,32 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" customWidth="1"/>
-    <col min="5" max="5" width="43.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.29296875" customWidth="1"/>
+    <col min="3" max="3" width="25.5859375" customWidth="1"/>
+    <col min="4" max="4" width="32.29296875" customWidth="1"/>
+    <col min="5" max="5" width="43.1171875" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="49.42578125" customWidth="1"/>
-    <col min="9" max="9" width="51.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23.87890625" customWidth="1"/>
+    <col min="8" max="8" width="49.41015625" customWidth="1"/>
+    <col min="9" max="9" width="51.29296875" customWidth="1"/>
     <col min="10" max="10" width="55" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="67.140625" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
-    <col min="14" max="14" width="50.7109375" customWidth="1"/>
+    <col min="12" max="12" width="67.1171875" customWidth="1"/>
+    <col min="13" max="13" width="19.1171875" customWidth="1"/>
+    <col min="14" max="14" width="50.703125" customWidth="1"/>
     <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="102.85546875" customWidth="1"/>
+    <col min="16" max="16" width="102.87890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -7498,7 +7641,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>265</v>
       </c>
@@ -7536,7 +7679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>262</v>
       </c>
@@ -7574,7 +7717,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -7621,7 +7764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -7647,7 +7790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>92</v>
       </c>
@@ -7691,7 +7834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -7729,7 +7872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -7773,7 +7916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>406</v>
       </c>
@@ -7811,7 +7954,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>226</v>
       </c>
@@ -7831,7 +7974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>225</v>
       </c>
@@ -7860,7 +8003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>401</v>
       </c>
@@ -7886,7 +8029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -7921,7 +8064,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>319</v>
       </c>
@@ -7944,7 +8087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -7979,7 +8122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -8011,7 +8154,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>375</v>
       </c>
@@ -8037,7 +8180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -8069,7 +8212,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -8107,7 +8250,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -8139,7 +8282,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>172</v>
       </c>
@@ -8159,7 +8302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -8191,7 +8334,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>95</v>
       </c>
@@ -8232,7 +8375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>253</v>
       </c>
@@ -8264,7 +8407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>250</v>
       </c>
@@ -8293,7 +8436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -8325,7 +8468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>213</v>
       </c>
@@ -8357,7 +8500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -8389,7 +8532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>271</v>
       </c>
@@ -8424,7 +8567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -8456,7 +8599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>97</v>
       </c>
@@ -8485,7 +8628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -8523,7 +8666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>399</v>
       </c>
@@ -8552,7 +8695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -8584,7 +8727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -8616,7 +8759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>268</v>
       </c>
@@ -8645,7 +8788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -8680,7 +8823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>222</v>
       </c>
@@ -8712,7 +8855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
         <v>402</v>
       </c>
@@ -8747,7 +8890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -8782,7 +8925,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
         <v>379</v>
       </c>
@@ -8808,7 +8951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
         <v>220</v>
       </c>
@@ -8828,7 +8971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
         <v>338</v>
       </c>
@@ -8879,14 +9022,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.29296875" customWidth="1"/>
+    <col min="2" max="2" width="39.29296875" customWidth="1"/>
+    <col min="3" max="3" width="18.5859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>168</v>
       </c>
@@ -8897,7 +9040,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>170</v>
       </c>
@@ -8908,7 +9051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>171</v>
       </c>
@@ -8919,7 +9062,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>176</v>
       </c>
@@ -8930,7 +9073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>176</v>
       </c>
@@ -8941,7 +9084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>170</v>
       </c>
@@ -8952,7 +9095,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>175</v>
       </c>
@@ -8963,7 +9106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>221</v>
       </c>
@@ -8974,7 +9117,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>170</v>
       </c>
@@ -8985,7 +9128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>171</v>
       </c>
@@ -8996,7 +9139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>170</v>
       </c>
@@ -9007,7 +9150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>175</v>
       </c>
@@ -9034,12 +9177,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="2" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>186</v>
       </c>
@@ -9047,7 +9190,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -9055,7 +9198,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>170</v>
       </c>
@@ -9063,7 +9206,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>175</v>
       </c>
@@ -9071,7 +9214,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>176</v>
       </c>
@@ -9079,7 +9222,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>221</v>
       </c>
@@ -9087,7 +9230,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>227</v>
       </c>
@@ -9107,37 +9250,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="0.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" customWidth="1"/>
-    <col min="11" max="11" width="4.140625" customWidth="1"/>
-    <col min="12" max="12" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="0.703125" customWidth="1"/>
+    <col min="3" max="3" width="13.703125" customWidth="1"/>
+    <col min="4" max="4" width="3.1171875" customWidth="1"/>
+    <col min="5" max="5" width="36.87890625" customWidth="1"/>
+    <col min="6" max="6" width="15.41015625" customWidth="1"/>
+    <col min="7" max="7" width="2.87890625" customWidth="1"/>
+    <col min="8" max="8" width="2.29296875" customWidth="1"/>
+    <col min="9" max="9" width="6.703125" customWidth="1"/>
+    <col min="10" max="10" width="4.41015625" customWidth="1"/>
+    <col min="11" max="11" width="4.1171875" customWidth="1"/>
+    <col min="12" max="12" width="3.29296875" customWidth="1"/>
     <col min="13" max="13" width="4" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" customWidth="1"/>
-    <col min="15" max="15" width="19.85546875" customWidth="1"/>
-    <col min="16" max="16" width="95.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.85546875" customWidth="1"/>
+    <col min="14" max="14" width="5.29296875" customWidth="1"/>
+    <col min="15" max="15" width="19.87890625" customWidth="1"/>
+    <col min="16" max="16" width="95.1171875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.87890625" customWidth="1"/>
     <col min="18" max="18" width="3" customWidth="1"/>
-    <col min="19" max="19" width="2.28515625" customWidth="1"/>
+    <col min="19" max="19" width="2.29296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -9196,7 +9339,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -9225,7 +9368,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>230</v>
       </c>
@@ -9254,7 +9397,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -9277,7 +9420,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>232</v>
       </c>
@@ -9305,7 +9448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>233</v>
       </c>
@@ -9328,7 +9471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>242</v>
       </c>
@@ -9351,7 +9494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>244</v>
       </c>
@@ -9374,7 +9517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>304</v>
       </c>
@@ -9397,7 +9540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>235</v>
       </c>
@@ -9423,7 +9566,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>179</v>
       </c>
@@ -9446,7 +9589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>248</v>
       </c>
@@ -9469,7 +9612,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>340</v>
       </c>
@@ -9489,7 +9632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>312</v>
       </c>
@@ -9512,7 +9655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>172</v>
       </c>
@@ -9526,7 +9669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>178</v>
       </c>

</xml_diff>